<commit_message>
added ci yml file
</commit_message>
<xml_diff>
--- a/src/test/resources/data/test_data.xlsx
+++ b/src/test/resources/data/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Demo_Projects\AutoScripter\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20E28CE-495A-475F-9721-AF09D1242E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8687E2D3-A32F-4317-9656-8B52C0A1608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BAA6C50-41BF-4B92-9008-7C9096EB3E7C}"/>
+    <workbookView xWindow="348" yWindow="360" windowWidth="17280" windowHeight="8964" xr2:uid="{5BAA6C50-41BF-4B92-9008-7C9096EB3E7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Test_Name</t>
   </si>
@@ -90,6 +89,27 @@
   </si>
   <si>
     <t>Verify Admin Page with valid data</t>
+  </si>
+  <si>
+    <t>searchPageTestValidData</t>
+  </si>
+  <si>
+    <t>Verify Search Page</t>
+  </si>
+  <si>
+    <t>User_Role</t>
+  </si>
+  <si>
+    <t>Employee_Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>User_Name</t>
+  </si>
+  <si>
+    <t>Enabled</t>
   </si>
 </sst>
 </file>
@@ -480,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5D1C56-FC4B-4AE5-AFDB-E50B0D63002E}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,10 +514,14 @@
     <col min="4" max="4" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,8 +540,20 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -537,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -557,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -575,6 +611,35 @@
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>